<commit_message>
Build site at 2022-06-20 16:07:16 UTC
</commit_message>
<xml_diff>
--- a/assets/disciplinas/LOM3202.xlsx
+++ b/assets/disciplinas/LOM3202.xlsx
@@ -134,11 +134,11 @@
     <t>Requisitos:</t>
   </si>
   <si>
+    <t xml:space="preserve">LOM3254 -  Laboratório de Circuitos Elétricos  (Indicação de Conjunto)
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">LOB1053 -  Física III  (Requisito)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOM3254 -  Laboratório de Circuitos Elétricos  (Indicação de Conjunto)
 </t>
   </si>
 </sst>

</xml_diff>

<commit_message>
Build site at 2022-06-24 16:07:18 UTC
</commit_message>
<xml_diff>
--- a/assets/disciplinas/LOM3202.xlsx
+++ b/assets/disciplinas/LOM3202.xlsx
@@ -134,11 +134,11 @@
     <t>Requisitos:</t>
   </si>
   <si>
+    <t xml:space="preserve">LOB1053 -  Física III  (Requisito)
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">LOM3254 -  Laboratório de Circuitos Elétricos  (Indicação de Conjunto)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOB1053 -  Física III  (Requisito)
 </t>
   </si>
 </sst>

</xml_diff>